<commit_message>
TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen - Final - 31 Mar 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen.xlsx
+++ b/TestData/TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AF9471-FC5B-47F3-9290-7B5DC4983F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E0DA6D-EB5D-47DA-94A9-AD2A8CA4690C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -270,10 +270,10 @@
     <t>Formal Pitch</t>
   </si>
   <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>Africa</t>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Benelux</t>
   </si>
 </sst>
 </file>
@@ -959,7 +959,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Opp Final - 31 Mar 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen.xlsx
+++ b/TestData/TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E0DA6D-EB5D-47DA-94A9-AD2A8CA4690C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FF51CF-6488-4330-96A1-33E2B73EF8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -252,9 +252,6 @@
     <t>Mark Martin</t>
   </si>
   <si>
-    <t>Rachell Schaller</t>
-  </si>
-  <si>
     <t>FSCO User</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>Benelux</t>
+  </si>
+  <si>
+    <t>Rachel Schaller</t>
   </si>
 </sst>
 </file>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +624,7 @@
         <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -632,7 +632,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -958,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01CAA37-8A09-4C20-87A8-FA8EE6CE15FC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
@@ -971,24 +971,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen - Final - 1 Apr 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen.xlsx
+++ b/TestData/TMTT0042712_VerificationOfBuyersListFeatureOnOpportunityScreen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FF51CF-6488-4330-96A1-33E2B73EF8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176B8D4D-6A1F-4383-A03C-7B6526129881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="468" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>Subject</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>Rachel Schaller</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>StandardTestCompany</t>
   </si>
 </sst>
 </file>
@@ -609,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -956,10 +962,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01CAA37-8A09-4C20-87A8-FA8EE6CE15FC}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,7 +975,7 @@
     <col min="3" max="3" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>71</v>
       </c>
@@ -979,8 +985,11 @@
       <c r="C1" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -989,6 +998,9 @@
       </c>
       <c r="C2" t="s">
         <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>